<commit_message>
work on 290 outline started
</commit_message>
<xml_diff>
--- a/CTEC290975JSWalleyspring2024.xlsx
+++ b/CTEC290975JSWalleyspring2024.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">Your Name </t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">Week 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am somewhat familiar with Mod 11: Methods of Securing Information</t>
   </si>
   <si>
     <t xml:space="preserve">Week 7</t>
@@ -224,40 +227,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -513,243 +520,245 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="69.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="68.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="73.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="3" t="s">
+    <row r="11" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5"/>
+      <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+    <row r="12" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+      <c r="B17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="n">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B29" s="6"/>
-    </row>
-    <row r="30" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="n">
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B30" s="6"/>
-    </row>
-    <row r="31" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="n">
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B31" s="6"/>
-    </row>
-    <row r="32" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="n">
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="B32" s="6"/>
+      <c r="B32" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
work on 290 finals completed
</commit_message>
<xml_diff>
--- a/CTEC290975JSWalleyspring2024.xlsx
+++ b/CTEC290975JSWalleyspring2024.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t xml:space="preserve">Your Name </t>
   </si>
@@ -82,49 +82,112 @@
     <t xml:space="preserve">Week 1</t>
   </si>
   <si>
+    <t xml:space="preserve">I learned what a MIS (Management Information System) is; I had never heard of one before.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I was not aware this was going to be a business class and I have no college business background.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go in knowing it is a business / technology class.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Week 2</t>
   </si>
   <si>
+    <t xml:space="preserve">I was familiar with the Cybersecurity information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I scored worse on the Cybersecurity section of this week’s learning material. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep up with the coursework. Some of the adaptive learning sections take a little time.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Week 3</t>
   </si>
   <si>
+    <t xml:space="preserve">Computer Networking is what I thought this class was about primarily.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a lot of information covered very quickly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plow through, there is a lot of information, but it is mostly good information.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Week 4</t>
   </si>
   <si>
+    <t xml:space="preserve">We are covering relatively current information in this course.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am focusing more on computer networks and less with business management.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This class gives a good overview of many broad topics. Take it in, good learning for a business setting.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Week 5</t>
   </si>
   <si>
+    <t xml:space="preserve">I am somewhat familiar with Mod 11: Methods of Securing Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yikes, like the cybersecurity section above, I did worse on the Securing Information section than the others.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep good notes of the terms in this course, they help clarify and define key aspects of modern enterprise.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Week 6</t>
   </si>
   <si>
-    <t xml:space="preserve">I am somewhat familiar with Mod 11: Methods of Securing Information</t>
+    <t xml:space="preserve">The information in this section was all pretty new to me and the software sounds fascinating.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I will most likely never get to truly utilize some of this Enterprise Resource software.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Break the work up into multiple days with this course. </t>
   </si>
   <si>
     <t xml:space="preserve">Week 7</t>
   </si>
   <si>
+    <t xml:space="preserve">I have never understood some of those finance concepts as well as I do now.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have no idea about anything to do with finance (but I learned some)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can realistically do at least 1 module and assignments per day if you work on it. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Week 8</t>
   </si>
   <si>
-    <t xml:space="preserve">Week 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week 14</t>
+    <t xml:space="preserve">I did great on the Computer hardware / software sections of the final.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Now I’ve got to go and pass this Math class so I can graduate and get back to the workforce.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you have never been in a real business environment, this class covers many concepts that you will need.</t>
   </si>
   <si>
     <t xml:space="preserve">List 4 things you would suggest to another student about taking this course.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a Business / Management and Technology course, not a designing computer networks class. I should have read the course description when talking to my advisor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a lot of information covered very quickly in this class. Make some notes, because there are relevant topics for a wide variety of topics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you do a little work in this class everyday it is not difficult. If you try to rush through 9+ exercises in 1 day it will be more difficult.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are some online Role Playing exercises in this course that I had fun doing. Hopefully one of the exercises will appeal to your learning style, also. </t>
   </si>
 </sst>
 </file>
@@ -134,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +227,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -227,7 +296,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,11 +325,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -519,16 +592,16 @@
   </sheetPr>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="69.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="68.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="73.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="83.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="92.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="92.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.42"/>
   </cols>
   <sheetData>
@@ -619,146 +692,188 @@
       <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="17" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="18" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="19" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="20" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
     </row>
     <row r="21" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
     </row>
     <row r="22" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="A22" s="0"/>
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
+      <c r="D22" s="0"/>
     </row>
     <row r="23" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="A23" s="0"/>
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
     </row>
     <row r="24" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="A24" s="0"/>
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
     </row>
     <row r="25" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
     </row>
     <row r="26" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
-        <v>34</v>
+      <c r="A28" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="n">
+      <c r="A29" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B29" s="7"/>
+      <c r="B29" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="30" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="n">
+      <c r="A30" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="31" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="n">
+      <c r="A31" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="32" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="n">
+      <c r="A32" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="B32" s="7"/>
+      <c r="B32" s="7" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>